<commit_message>
Update data files and HTML reports - Improve schedule autofill script with enhanced port name mapping and HTML extraction logic
</commit_message>
<xml_diff>
--- a/Data/Market-SCFI-Trends.xlsx
+++ b/Data/Market-SCFI-Trends.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29712"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9743FB03-5A23-462F-B07A-98CD9E27E145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EF9422-D1D2-467B-89E6-1CD1824D24A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13560" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,13 +532,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S814"/>
+  <dimension ref="A1:S815"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B779" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B775" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A814" sqref="A814"/>
+      <selection pane="bottomRight" activeCell="A815" sqref="A815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -43505,53 +43505,106 @@
       <c r="A814" s="6">
         <v>46031</v>
       </c>
-      <c r="B814" s="11">
+      <c r="B814" s="10">
         <v>1647.39</v>
       </c>
-      <c r="C814" s="11">
+      <c r="C814" s="10">
         <v>1281</v>
       </c>
-      <c r="D814" s="11">
+      <c r="D814" s="10">
         <v>321</v>
       </c>
-      <c r="E814" s="11">
+      <c r="E814" s="10">
         <v>2094</v>
       </c>
-      <c r="F814" s="11">
+      <c r="F814" s="10">
         <v>3128</v>
       </c>
-      <c r="G814" s="11">
+      <c r="G814" s="10">
         <v>1719</v>
       </c>
-      <c r="H814" s="11">
+      <c r="H814" s="10">
         <v>142</v>
       </c>
-      <c r="I814" s="11">
+      <c r="I814" s="10">
         <v>3232</v>
       </c>
-      <c r="J814" s="11">
+      <c r="J814" s="10">
         <v>1981</v>
       </c>
-      <c r="K814" s="11">
+      <c r="K814" s="10">
         <v>2407</v>
       </c>
-      <c r="L814" s="11">
+      <c r="L814" s="10">
         <v>1208</v>
       </c>
-      <c r="M814" s="11">
+      <c r="M814" s="10">
         <v>524</v>
       </c>
-      <c r="N814" s="11">
+      <c r="N814" s="10">
         <v>3264</v>
       </c>
-      <c r="O814" s="11">
+      <c r="O814" s="10">
         <v>312</v>
       </c>
-      <c r="P814" s="11">
+      <c r="P814" s="10">
         <v>2218</v>
       </c>
-      <c r="Q814" s="11">
+      <c r="Q814" s="10">
         <v>1026</v>
+      </c>
+    </row>
+    <row r="815" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A815" s="6">
+        <v>46038</v>
+      </c>
+      <c r="B815" s="11">
+        <v>1574.12</v>
+      </c>
+      <c r="C815" s="11">
+        <v>1151</v>
+      </c>
+      <c r="D815" s="11">
+        <v>321</v>
+      </c>
+      <c r="E815" s="11">
+        <v>1953</v>
+      </c>
+      <c r="F815" s="11">
+        <v>3165</v>
+      </c>
+      <c r="G815" s="11">
+        <v>1676</v>
+      </c>
+      <c r="H815" s="11">
+        <v>144</v>
+      </c>
+      <c r="I815" s="11">
+        <v>2983</v>
+      </c>
+      <c r="J815" s="11">
+        <v>1694</v>
+      </c>
+      <c r="K815" s="11">
+        <v>2259</v>
+      </c>
+      <c r="L815" s="11">
+        <v>1195</v>
+      </c>
+      <c r="M815" s="11">
+        <v>515</v>
+      </c>
+      <c r="N815" s="11">
+        <v>3192</v>
+      </c>
+      <c r="O815" s="11">
+        <v>312</v>
+      </c>
+      <c r="P815" s="11">
+        <v>2194</v>
+      </c>
+      <c r="Q815" s="11">
+        <v>1001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add customer highlight feature in VSL/VOY + Limit mode
- Add orange highlight for rows where customer percentage exceeds 15% and GPS is low
- Add AVG GPS column in detail modal for easy comparison
- Implement three-condition check: customer percentage > 15%, allocation check (if available), and GPS comparison
- Update Excel data files for market analysis and trends
</commit_message>
<xml_diff>
--- a/Data/Market-SCFI-Trends.xlsx
+++ b/Data/Market-SCFI-Trends.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29713"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EF9422-D1D2-467B-89E6-1CD1824D24A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8E1094-7CEB-4A56-A27A-EEB981AEACE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13560" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,13 +532,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S815"/>
+  <dimension ref="A1:S816"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B775" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B793" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A815" sqref="A815"/>
+      <selection pane="bottomRight" activeCell="A816" sqref="A816"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -43558,53 +43558,106 @@
       <c r="A815" s="6">
         <v>46038</v>
       </c>
-      <c r="B815" s="11">
+      <c r="B815" s="10">
         <v>1574.12</v>
       </c>
-      <c r="C815" s="11">
+      <c r="C815" s="10">
         <v>1151</v>
       </c>
-      <c r="D815" s="11">
+      <c r="D815" s="10">
         <v>321</v>
       </c>
-      <c r="E815" s="11">
+      <c r="E815" s="10">
         <v>1953</v>
       </c>
-      <c r="F815" s="11">
+      <c r="F815" s="10">
         <v>3165</v>
       </c>
-      <c r="G815" s="11">
+      <c r="G815" s="10">
         <v>1676</v>
       </c>
-      <c r="H815" s="11">
+      <c r="H815" s="10">
         <v>144</v>
       </c>
-      <c r="I815" s="11">
+      <c r="I815" s="10">
         <v>2983</v>
       </c>
-      <c r="J815" s="11">
+      <c r="J815" s="10">
         <v>1694</v>
       </c>
-      <c r="K815" s="11">
+      <c r="K815" s="10">
         <v>2259</v>
       </c>
-      <c r="L815" s="11">
+      <c r="L815" s="10">
         <v>1195</v>
       </c>
-      <c r="M815" s="11">
+      <c r="M815" s="10">
         <v>515</v>
       </c>
-      <c r="N815" s="11">
+      <c r="N815" s="10">
         <v>3192</v>
       </c>
-      <c r="O815" s="11">
+      <c r="O815" s="10">
         <v>312</v>
       </c>
-      <c r="P815" s="11">
+      <c r="P815" s="10">
         <v>2194</v>
       </c>
-      <c r="Q815" s="11">
+      <c r="Q815" s="10">
         <v>1001</v>
+      </c>
+    </row>
+    <row r="816" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A816" s="6">
+        <v>46045</v>
+      </c>
+      <c r="B816" s="11">
+        <v>1457.86</v>
+      </c>
+      <c r="C816" s="11">
+        <v>1029</v>
+      </c>
+      <c r="D816" s="11">
+        <v>321</v>
+      </c>
+      <c r="E816" s="11">
+        <v>1842</v>
+      </c>
+      <c r="F816" s="11">
+        <v>2896</v>
+      </c>
+      <c r="G816" s="11">
+        <v>1595</v>
+      </c>
+      <c r="H816" s="11">
+        <v>144</v>
+      </c>
+      <c r="I816" s="11">
+        <v>2756</v>
+      </c>
+      <c r="J816" s="11">
+        <v>1288</v>
+      </c>
+      <c r="K816" s="11">
+        <v>2144</v>
+      </c>
+      <c r="L816" s="11">
+        <v>1153</v>
+      </c>
+      <c r="M816" s="11">
+        <v>496</v>
+      </c>
+      <c r="N816" s="11">
+        <v>3141</v>
+      </c>
+      <c r="O816" s="11">
+        <v>312</v>
+      </c>
+      <c r="P816" s="11">
+        <v>2084</v>
+      </c>
+      <c r="Q816" s="11">
+        <v>939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update market data: 001-03-market-analysis, 365-03-market-watch, Market-SCFI-Trends
</commit_message>
<xml_diff>
--- a/Data/Market-SCFI-Trends.xlsx
+++ b/Data/Market-SCFI-Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8E1094-7CEB-4A56-A27A-EEB981AEACE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667679C5-7C9D-47C9-8FE7-B65958BE4F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13560" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIN Timeseries - W" sheetId="2" r:id="rId1"/>
@@ -532,13 +532,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S816"/>
+  <dimension ref="A1:S817"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B793" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B805" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A816" sqref="A816"/>
+      <selection pane="bottomRight" activeCell="A817" sqref="A817"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -43611,53 +43611,106 @@
       <c r="A816" s="6">
         <v>46045</v>
       </c>
-      <c r="B816" s="11">
+      <c r="B816" s="10">
         <v>1457.86</v>
       </c>
-      <c r="C816" s="11">
+      <c r="C816" s="10">
         <v>1029</v>
       </c>
-      <c r="D816" s="11">
+      <c r="D816" s="10">
         <v>321</v>
       </c>
-      <c r="E816" s="11">
+      <c r="E816" s="10">
         <v>1842</v>
       </c>
-      <c r="F816" s="11">
+      <c r="F816" s="10">
         <v>2896</v>
       </c>
-      <c r="G816" s="11">
+      <c r="G816" s="10">
         <v>1595</v>
       </c>
-      <c r="H816" s="11">
+      <c r="H816" s="10">
         <v>144</v>
       </c>
-      <c r="I816" s="11">
+      <c r="I816" s="10">
         <v>2756</v>
       </c>
-      <c r="J816" s="11">
+      <c r="J816" s="10">
         <v>1288</v>
       </c>
-      <c r="K816" s="11">
+      <c r="K816" s="10">
         <v>2144</v>
       </c>
-      <c r="L816" s="11">
+      <c r="L816" s="10">
         <v>1153</v>
       </c>
-      <c r="M816" s="11">
+      <c r="M816" s="10">
         <v>496</v>
       </c>
-      <c r="N816" s="11">
+      <c r="N816" s="10">
         <v>3141</v>
       </c>
-      <c r="O816" s="11">
+      <c r="O816" s="10">
         <v>312</v>
       </c>
-      <c r="P816" s="11">
+      <c r="P816" s="10">
         <v>2084</v>
       </c>
-      <c r="Q816" s="11">
+      <c r="Q816" s="10">
         <v>939</v>
+      </c>
+    </row>
+    <row r="817" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A817" s="6">
+        <v>46052</v>
+      </c>
+      <c r="B817" s="11">
+        <v>1316.75</v>
+      </c>
+      <c r="C817" s="11">
+        <v>870</v>
+      </c>
+      <c r="D817" s="11">
+        <v>321</v>
+      </c>
+      <c r="E817" s="11">
+        <v>1744</v>
+      </c>
+      <c r="F817" s="11">
+        <v>2605</v>
+      </c>
+      <c r="G817" s="11">
+        <v>1418</v>
+      </c>
+      <c r="H817" s="11">
+        <v>144</v>
+      </c>
+      <c r="I817" s="11">
+        <v>2424</v>
+      </c>
+      <c r="J817" s="11">
+        <v>997</v>
+      </c>
+      <c r="K817" s="11">
+        <v>2059</v>
+      </c>
+      <c r="L817" s="11">
+        <v>1131</v>
+      </c>
+      <c r="M817" s="11">
+        <v>483</v>
+      </c>
+      <c r="N817" s="11">
+        <v>3074</v>
+      </c>
+      <c r="O817" s="11">
+        <v>312</v>
+      </c>
+      <c r="P817" s="11">
+        <v>1867</v>
+      </c>
+      <c r="Q817" s="11">
+        <v>877</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: market analysis, SCFI trends, booking summaries, parsed ports list
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/Data/Market-SCFI-Trends.xlsx
+++ b/Data/Market-SCFI-Trends.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29803"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Applications\Cursor\Shipping Schedule\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667679C5-7C9D-47C9-8FE7-B65958BE4F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE5E5B3-D075-4051-BDAE-B773066F2CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13560" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIN Timeseries - W" sheetId="2" r:id="rId1"/>
@@ -532,13 +532,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S817"/>
+  <dimension ref="A1:S818"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B805" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A817" sqref="A817"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -43664,53 +43664,106 @@
       <c r="A817" s="6">
         <v>46052</v>
       </c>
-      <c r="B817" s="11">
+      <c r="B817" s="10">
         <v>1316.75</v>
       </c>
-      <c r="C817" s="11">
+      <c r="C817" s="10">
         <v>870</v>
       </c>
-      <c r="D817" s="11">
+      <c r="D817" s="10">
         <v>321</v>
       </c>
-      <c r="E817" s="11">
+      <c r="E817" s="10">
         <v>1744</v>
       </c>
-      <c r="F817" s="11">
+      <c r="F817" s="10">
         <v>2605</v>
       </c>
-      <c r="G817" s="11">
+      <c r="G817" s="10">
         <v>1418</v>
       </c>
-      <c r="H817" s="11">
+      <c r="H817" s="10">
         <v>144</v>
       </c>
-      <c r="I817" s="11">
+      <c r="I817" s="10">
         <v>2424</v>
       </c>
-      <c r="J817" s="11">
+      <c r="J817" s="10">
         <v>997</v>
       </c>
-      <c r="K817" s="11">
+      <c r="K817" s="10">
         <v>2059</v>
       </c>
-      <c r="L817" s="11">
+      <c r="L817" s="10">
         <v>1131</v>
       </c>
-      <c r="M817" s="11">
+      <c r="M817" s="10">
         <v>483</v>
       </c>
-      <c r="N817" s="11">
+      <c r="N817" s="10">
         <v>3074</v>
       </c>
-      <c r="O817" s="11">
+      <c r="O817" s="10">
         <v>312</v>
       </c>
-      <c r="P817" s="11">
+      <c r="P817" s="10">
         <v>1867</v>
       </c>
-      <c r="Q817" s="11">
+      <c r="Q817" s="10">
         <v>877</v>
+      </c>
+    </row>
+    <row r="818" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A818" s="6">
+        <v>46059</v>
+      </c>
+      <c r="B818" s="11">
+        <v>1266.56</v>
+      </c>
+      <c r="C818" s="11">
+        <v>745</v>
+      </c>
+      <c r="D818" s="11">
+        <v>321</v>
+      </c>
+      <c r="E818" s="11">
+        <v>1693</v>
+      </c>
+      <c r="F818" s="11">
+        <v>2530</v>
+      </c>
+      <c r="G818" s="11">
+        <v>1403</v>
+      </c>
+      <c r="H818" s="11">
+        <v>139</v>
+      </c>
+      <c r="I818" s="11">
+        <v>2291</v>
+      </c>
+      <c r="J818" s="11">
+        <v>917</v>
+      </c>
+      <c r="K818" s="11">
+        <v>1938</v>
+      </c>
+      <c r="L818" s="11">
+        <v>1136</v>
+      </c>
+      <c r="M818" s="11">
+        <v>461</v>
+      </c>
+      <c r="N818" s="11">
+        <v>3024</v>
+      </c>
+      <c r="O818" s="11">
+        <v>312</v>
+      </c>
+      <c r="P818" s="11">
+        <v>1801</v>
+      </c>
+      <c r="Q818" s="11">
+        <v>932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>